<commit_message>
memperbaiki import data mahasiswa tanpa header
</commit_message>
<xml_diff>
--- a/si-mhsdo/public/MahasiswaData/daftarmahasiswa (1).xlsx
+++ b/si-mhsdo/public/MahasiswaData/daftarmahasiswa (1).xlsx
@@ -1,37 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\This Pc\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="162913" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Nama_Mahasiswa</t>
-  </si>
-  <si>
     <t>NIM</t>
   </si>
   <si>
-    <t>Tahun_Angkatan</t>
-  </si>
-  <si>
-    <t>Program_studi</t>
-  </si>
-  <si>
     <t>Fakultas</t>
   </si>
   <si>
@@ -47,12 +42,6 @@
     <t>Masa_Studi</t>
   </si>
   <si>
-    <t>NoHP_Ortu</t>
-  </si>
-  <si>
-    <t>NoHP_Mahasiswa</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -198,19 +187,29 @@
   </si>
   <si>
     <t>elfijariodqalbi@gmail.com</t>
+  </si>
+  <si>
+    <t>angkatan</t>
+  </si>
+  <si>
+    <t>Prodi</t>
+  </si>
+  <si>
+    <t>HP_Ortu</t>
+  </si>
+  <si>
+    <t>HP_Mahasiswa</t>
+  </si>
+  <si>
+    <t>nama-mahasiswa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -225,21 +224,33 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -286,7 +297,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -321,7 +332,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -529,71 +540,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1911522012</v>
@@ -602,10 +610,10 @@
         <v>2019</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>7</v>
@@ -620,27 +628,27 @@
         <v>123</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>2222222222</v>
@@ -649,10 +657,10 @@
         <v>2019</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G3">
         <v>13</v>
@@ -664,30 +672,30 @@
         <v>43</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>1911521021</v>
@@ -696,10 +704,10 @@
         <v>2019</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>7</v>
@@ -711,30 +719,30 @@
         <v>43</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>1111111111</v>
@@ -743,45 +751,45 @@
         <v>2019</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G5">
         <v>7</v>
       </c>
       <c r="H5">
-        <v>2.22</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="I5">
         <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="M5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="N5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>1911523023</v>
@@ -790,45 +798,45 @@
         <v>2019</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>7</v>
       </c>
       <c r="H6">
-        <v>2.22</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="I6">
         <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="N6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>91525512</v>
@@ -837,10 +845,10 @@
         <v>2019</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G7">
         <v>7</v>
@@ -852,30 +860,30 @@
         <v>100</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="M7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="N7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <v>1911522012</v>
@@ -884,10 +892,10 @@
         <v>2019</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -902,27 +910,27 @@
         <v>123</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="L8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="M8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>1911522012</v>
@@ -931,16 +939,16 @@
         <v>2019</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="I9">
         <v>100</v>
@@ -949,27 +957,27 @@
         <v>7.5</v>
       </c>
       <c r="K9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C10">
         <v>2222222222</v>
@@ -978,16 +986,16 @@
         <v>2019</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G10">
         <v>13</v>
       </c>
       <c r="H10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="I10">
         <v>100</v>
@@ -996,33 +1004,22 @@
         <v>7.5</v>
       </c>
       <c r="K10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="L10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update query dashboard dan tampilan status evaluasi
</commit_message>
<xml_diff>
--- a/si-mhsdo/public/MahasiswaData/daftarmahasiswa (1).xlsx
+++ b/si-mhsdo/public/MahasiswaData/daftarmahasiswa (1).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="63">
   <si>
     <t>No</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Total_SKS</t>
   </si>
   <si>
-    <t>Masa_Studi</t>
-  </si>
-  <si>
     <t>HP_Ortu</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Evaluasi</t>
-  </si>
-  <si>
     <t>Alex Putra Siregar</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>aktif</t>
   </si>
   <si>
-    <t>terancam do</t>
-  </si>
-  <si>
     <t>Elfijario Direnda Qalbi</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
   </si>
   <si>
     <t>Aminah</t>
-  </si>
-  <si>
-    <t>aman</t>
   </si>
   <si>
     <t>Ricky Akbar</t>
@@ -551,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +552,7 @@
     <col min="6" max="6" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,19 +592,13 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1911523099</v>
@@ -625,10 +607,10 @@
         <v>2021</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -639,31 +621,25 @@
       <c r="I2">
         <v>60</v>
       </c>
-      <c r="J2">
-        <v>3</v>
+      <c r="J2" t="s">
+        <v>14</v>
       </c>
       <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
       <c r="M2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>1911521021</v>
@@ -672,10 +648,10 @@
         <v>2019</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G3">
         <v>13</v>
@@ -686,31 +662,25 @@
       <c r="I3">
         <v>150</v>
       </c>
-      <c r="J3">
-        <v>6</v>
+      <c r="J3" t="s">
+        <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>1911523111</v>
@@ -719,10 +689,10 @@
         <v>2017</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G4">
         <v>13</v>
@@ -733,31 +703,25 @@
       <c r="I4">
         <v>149</v>
       </c>
-      <c r="J4">
-        <v>7</v>
+      <c r="J4" t="s">
+        <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>1911522007</v>
@@ -766,10 +730,10 @@
         <v>2019</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G5">
         <v>13</v>
@@ -780,31 +744,25 @@
       <c r="I5">
         <v>111</v>
       </c>
-      <c r="J5">
-        <v>7</v>
+      <c r="J5" t="s">
+        <v>24</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>1911523025</v>
@@ -813,10 +771,10 @@
         <v>2019</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G6">
         <v>13</v>
@@ -827,31 +785,25 @@
       <c r="I6">
         <v>122</v>
       </c>
-      <c r="J6">
-        <v>7</v>
+      <c r="J6" t="s">
+        <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="M6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>1911523099</v>
@@ -860,10 +812,10 @@
         <v>2021</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -874,31 +826,25 @@
       <c r="I7">
         <v>55</v>
       </c>
-      <c r="J7">
-        <v>3</v>
+      <c r="J7" t="s">
+        <v>14</v>
       </c>
       <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
         <v>16</v>
       </c>
-      <c r="L7" t="s">
-        <v>17</v>
-      </c>
       <c r="M7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>1911521021</v>
@@ -907,10 +853,10 @@
         <v>2019</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G8">
         <v>13</v>
@@ -921,31 +867,25 @@
       <c r="I8">
         <v>150</v>
       </c>
-      <c r="J8">
-        <v>6</v>
+      <c r="J8" t="s">
+        <v>19</v>
       </c>
       <c r="K8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M8" t="s">
-        <v>24</v>
-      </c>
-      <c r="N8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>1911523111</v>
@@ -954,10 +894,10 @@
         <v>2017</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G9">
         <v>13</v>
@@ -968,31 +908,25 @@
       <c r="I9">
         <v>149</v>
       </c>
-      <c r="J9">
-        <v>7</v>
+      <c r="J9" t="s">
+        <v>24</v>
       </c>
       <c r="K9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>1911522007</v>
@@ -1001,10 +935,10 @@
         <v>2019</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -1015,31 +949,25 @@
       <c r="I10">
         <v>40</v>
       </c>
-      <c r="J10">
-        <v>3</v>
+      <c r="J10" t="s">
+        <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M10" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <v>1911523025</v>
@@ -1048,10 +976,10 @@
         <v>2016</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G11">
         <v>13</v>
@@ -1062,31 +990,25 @@
       <c r="I11">
         <v>122</v>
       </c>
-      <c r="J11">
-        <v>7</v>
+      <c r="J11" t="s">
+        <v>24</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L11" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="M11" t="s">
-        <v>32</v>
-      </c>
-      <c r="N11" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>1911591011</v>
@@ -1095,10 +1017,10 @@
         <v>2019</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G12">
         <v>13</v>
@@ -1109,31 +1031,25 @@
       <c r="I12">
         <v>121</v>
       </c>
-      <c r="J12">
-        <v>6.5</v>
+      <c r="J12" t="s">
+        <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M12" t="s">
-        <v>41</v>
-      </c>
-      <c r="N12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13">
         <v>1611523025</v>
@@ -1142,10 +1058,10 @@
         <v>2016</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -1154,33 +1070,27 @@
         <v>2.99</v>
       </c>
       <c r="I13">
-        <v>122</v>
-      </c>
-      <c r="J13">
-        <v>7.5</v>
+        <v>53</v>
+      </c>
+      <c r="J13" t="s">
+        <v>19</v>
       </c>
       <c r="K13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="M13" t="s">
-        <v>32</v>
-      </c>
-      <c r="N13" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C14">
         <v>1511431001</v>
@@ -1189,10 +1099,10 @@
         <v>2021</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G14">
         <v>3</v>
@@ -1201,33 +1111,27 @@
         <v>1.43</v>
       </c>
       <c r="I14">
-        <v>122</v>
-      </c>
-      <c r="J14">
-        <v>7.5</v>
+        <v>40</v>
+      </c>
+      <c r="J14" t="s">
+        <v>24</v>
       </c>
       <c r="K14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L14" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M14" t="s">
-        <v>44</v>
-      </c>
-      <c r="N14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>1911523099</v>
@@ -1236,10 +1140,10 @@
         <v>2021</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -1250,31 +1154,25 @@
       <c r="I15">
         <v>60</v>
       </c>
-      <c r="J15">
-        <v>3</v>
+      <c r="J15" t="s">
+        <v>14</v>
       </c>
       <c r="K15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" t="s">
         <v>16</v>
       </c>
-      <c r="L15" t="s">
-        <v>17</v>
-      </c>
       <c r="M15" t="s">
-        <v>18</v>
-      </c>
-      <c r="N15" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>1911521021</v>
@@ -1283,10 +1181,10 @@
         <v>2019</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G16">
         <v>13</v>
@@ -1297,31 +1195,25 @@
       <c r="I16">
         <v>150</v>
       </c>
-      <c r="J16">
-        <v>6</v>
+      <c r="J16" t="s">
+        <v>19</v>
       </c>
       <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
-      </c>
-      <c r="L16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" t="s">
-        <v>24</v>
-      </c>
-      <c r="N16" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
       </c>
       <c r="C17">
         <v>1911523111</v>
@@ -1330,10 +1222,10 @@
         <v>2017</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G17">
         <v>13</v>
@@ -1344,31 +1236,25 @@
       <c r="I17">
         <v>149</v>
       </c>
-      <c r="J17">
-        <v>7</v>
+      <c r="J17" t="s">
+        <v>24</v>
       </c>
       <c r="K17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M17" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C18">
         <v>1911522007</v>
@@ -1377,10 +1263,10 @@
         <v>2019</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G18">
         <v>13</v>
@@ -1391,31 +1277,25 @@
       <c r="I18">
         <v>111</v>
       </c>
-      <c r="J18">
-        <v>7</v>
+      <c r="J18" t="s">
+        <v>24</v>
       </c>
       <c r="K18" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="L18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M18" t="s">
-        <v>18</v>
-      </c>
-      <c r="N18" t="s">
-        <v>19</v>
-      </c>
-      <c r="O18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C19">
         <v>1911523025</v>
@@ -1424,10 +1304,10 @@
         <v>2019</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G19">
         <v>13</v>
@@ -1438,31 +1318,25 @@
       <c r="I19">
         <v>122</v>
       </c>
-      <c r="J19">
-        <v>7</v>
+      <c r="J19" t="s">
+        <v>24</v>
       </c>
       <c r="K19" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L19" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="M19" t="s">
-        <v>32</v>
-      </c>
-      <c r="N19" t="s">
-        <v>19</v>
-      </c>
-      <c r="O19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>1911523099</v>
@@ -1471,10 +1345,10 @@
         <v>2021</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G20">
         <v>3</v>
@@ -1485,31 +1359,25 @@
       <c r="I20">
         <v>55</v>
       </c>
-      <c r="J20">
-        <v>3</v>
+      <c r="J20" t="s">
+        <v>14</v>
       </c>
       <c r="K20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" t="s">
         <v>16</v>
       </c>
-      <c r="L20" t="s">
-        <v>17</v>
-      </c>
       <c r="M20" t="s">
-        <v>18</v>
-      </c>
-      <c r="N20" t="s">
-        <v>19</v>
-      </c>
-      <c r="O20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>1911521021</v>
@@ -1518,10 +1386,10 @@
         <v>2019</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G21">
         <v>13</v>
@@ -1532,31 +1400,25 @@
       <c r="I21">
         <v>150</v>
       </c>
-      <c r="J21">
-        <v>6</v>
+      <c r="J21" t="s">
+        <v>19</v>
       </c>
       <c r="K21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M21" t="s">
-        <v>24</v>
-      </c>
-      <c r="N21" t="s">
-        <v>19</v>
-      </c>
-      <c r="O21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>1911523111</v>
@@ -1565,10 +1427,10 @@
         <v>2017</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G22">
         <v>13</v>
@@ -1579,31 +1441,25 @@
       <c r="I22">
         <v>149</v>
       </c>
-      <c r="J22">
-        <v>7</v>
+      <c r="J22" t="s">
+        <v>24</v>
       </c>
       <c r="K22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M22" t="s">
-        <v>29</v>
-      </c>
-      <c r="N22" t="s">
-        <v>19</v>
-      </c>
-      <c r="O22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>1911522007</v>
@@ -1612,10 +1468,10 @@
         <v>2019</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G23">
         <v>3</v>
@@ -1626,31 +1482,25 @@
       <c r="I23">
         <v>40</v>
       </c>
-      <c r="J23">
-        <v>3</v>
+      <c r="J23" t="s">
+        <v>24</v>
       </c>
       <c r="K23" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="L23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M23" t="s">
-        <v>18</v>
-      </c>
-      <c r="N23" t="s">
-        <v>19</v>
-      </c>
-      <c r="O23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C24">
         <v>1911523025</v>
@@ -1659,10 +1509,10 @@
         <v>2016</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G24">
         <v>13</v>
@@ -1673,31 +1523,25 @@
       <c r="I24">
         <v>122</v>
       </c>
-      <c r="J24">
-        <v>7</v>
+      <c r="J24" t="s">
+        <v>24</v>
       </c>
       <c r="K24" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L24" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="M24" t="s">
-        <v>32</v>
-      </c>
-      <c r="N24" t="s">
-        <v>19</v>
-      </c>
-      <c r="O24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <v>1911591011</v>
@@ -1706,10 +1550,10 @@
         <v>2019</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G25">
         <v>13</v>
@@ -1720,31 +1564,25 @@
       <c r="I25">
         <v>121</v>
       </c>
-      <c r="J25">
-        <v>6.5</v>
+      <c r="J25" t="s">
+        <v>36</v>
       </c>
       <c r="K25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M25" t="s">
-        <v>41</v>
-      </c>
-      <c r="N25" t="s">
-        <v>19</v>
-      </c>
-      <c r="O25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C26">
         <v>1611523025</v>
@@ -1753,10 +1591,10 @@
         <v>2016</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G26">
         <v>3</v>
@@ -1765,33 +1603,27 @@
         <v>2.99</v>
       </c>
       <c r="I26">
-        <v>122</v>
-      </c>
-      <c r="J26">
-        <v>7.5</v>
+        <v>44</v>
+      </c>
+      <c r="J26" t="s">
+        <v>19</v>
       </c>
       <c r="K26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L26" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="M26" t="s">
-        <v>32</v>
-      </c>
-      <c r="N26" t="s">
-        <v>19</v>
-      </c>
-      <c r="O26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C27">
         <v>1511431001</v>
@@ -1800,10 +1632,10 @@
         <v>2021</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G27">
         <v>3</v>
@@ -1812,25 +1644,19 @@
         <v>1.43</v>
       </c>
       <c r="I27">
-        <v>122</v>
-      </c>
-      <c r="J27">
-        <v>7.5</v>
+        <v>31</v>
+      </c>
+      <c r="J27" t="s">
+        <v>24</v>
       </c>
       <c r="K27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L27" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M27" t="s">
-        <v>44</v>
-      </c>
-      <c r="N27" t="s">
-        <v>19</v>
-      </c>
-      <c r="O27" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>